<commit_message>
Driver file - result sheet is added with one more column failed functions
</commit_message>
<xml_diff>
--- a/src/com/styletag/test_cases/InputData.xlsx
+++ b/src/com/styletag/test_cases/InputData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t xml:space="preserve">Email ID</t>
   </si>
@@ -115,10 +115,13 @@
     <t xml:space="preserve">Login ID</t>
   </si>
   <si>
+    <t xml:space="preserve">test3456@styletag.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">styletag123</t>
+  </si>
+  <si>
     <t xml:space="preserve">test16@styletag.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">styletag123</t>
   </si>
   <si>
     <t xml:space="preserve">Search Keyword</t>
@@ -271,13 +274,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,16 +506,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,9 +539,15 @@
         <v>31</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="test16@styletag.com"/>
+    <hyperlink ref="A3" r:id="rId1" display="test3456@styletag.com"/>
+    <hyperlink ref="A12" r:id="rId2" display="test16@styletag.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -557,39 +566,38 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>